<commit_message>
account for label transfer
</commit_message>
<xml_diff>
--- a/nucleotide_salvage_tracing/Uridine-Hypoxanthine/output/143B_isotopologues-corrected.xlsx
+++ b/nucleotide_salvage_tracing/Uridine-Hypoxanthine/output/143B_isotopologues-corrected.xlsx
@@ -1059,7 +1059,7 @@
         <v>0.3290318940752242</v>
       </c>
       <c r="BO2">
-        <v>0.002450791451157539</v>
+        <v>0.00245079145115754</v>
       </c>
       <c r="BP2">
         <v>0.6867981514718746</v>
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="BW2">
-        <v>0.00117060922493675</v>
+        <v>0.001170609224936749</v>
       </c>
       <c r="BX2">
         <v>0.8258314174395998</v>
@@ -1307,13 +1307,13 @@
         <v>0.1591689821682241</v>
       </c>
       <c r="BS3">
-        <v>0.000138326812462653</v>
+        <v>0.0001383268165529389</v>
       </c>
       <c r="BT3">
-        <v>0.8606024549761095</v>
+        <v>0.8606024549777928</v>
       </c>
       <c r="BU3">
-        <v>0.1392592182114279</v>
+        <v>0.1392592182056543</v>
       </c>
       <c r="BV3">
         <v>0</v>
@@ -1322,13 +1322,13 @@
         <v>0</v>
       </c>
       <c r="BX3">
-        <v>0.904782106872803</v>
+        <v>0.9047821068648386</v>
       </c>
       <c r="BY3">
-        <v>0.09438576393333405</v>
+        <v>0.09438576393316397</v>
       </c>
       <c r="BZ3">
-        <v>0.0008321291938628817</v>
+        <v>0.000832129201997412</v>
       </c>
     </row>
     <row r="4" spans="1:78">
@@ -1495,7 +1495,7 @@
         <v>0.986831544446653</v>
       </c>
       <c r="BC4">
-        <v>0.000150308744610146</v>
+        <v>0.0001503087446101467</v>
       </c>
       <c r="BD4">
         <v>0.01301814680873681</v>
@@ -1555,13 +1555,13 @@
         <v>0</v>
       </c>
       <c r="BW4">
-        <v>0.0008946487240551805</v>
+        <v>0.0008946487240551808</v>
       </c>
       <c r="BX4">
         <v>0.9848534027310147</v>
       </c>
       <c r="BY4">
-        <v>0.01425194854493016</v>
+        <v>0.01425194854493017</v>
       </c>
       <c r="BZ4">
         <v>0</v>
@@ -1722,7 +1722,7 @@
         <v>0.9883099987234271</v>
       </c>
       <c r="AZ5">
-        <v>0.009261220876775007</v>
+        <v>0.009261220876775006</v>
       </c>
       <c r="BA5">
         <v>0.002428780399797895</v>
@@ -1785,7 +1785,7 @@
         <v>0.9895697924345449</v>
       </c>
       <c r="BU5">
-        <v>0.01043020756545512</v>
+        <v>0.01043020756545511</v>
       </c>
       <c r="BV5">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="AW6">
-        <v>0.005423340227695264</v>
+        <v>0.005423340227695263</v>
       </c>
       <c r="AX6">
         <v>0.9945766597723048</v>
@@ -1964,13 +1964,13 @@
         <v>0.00179581769030139</v>
       </c>
       <c r="BB6">
-        <v>0.9935981820818457</v>
+        <v>0.9935981820818771</v>
       </c>
       <c r="BC6">
         <v>0</v>
       </c>
       <c r="BD6">
-        <v>0.006401817918154203</v>
+        <v>0.006401817918122913</v>
       </c>
       <c r="BE6">
         <v>0.9840662447083965</v>
@@ -1985,13 +1985,13 @@
         <v>0.995851446417217</v>
       </c>
       <c r="BI6">
-        <v>0.004148553582783032</v>
+        <v>0.004148553582783033</v>
       </c>
       <c r="BJ6">
         <v>0</v>
       </c>
       <c r="BK6">
-        <v>0.007787608186081545</v>
+        <v>0.007787608186081541</v>
       </c>
       <c r="BL6">
         <v>0.9922123918139185</v>
@@ -2191,13 +2191,13 @@
         <v>0.9843657904366986</v>
       </c>
       <c r="AY7">
-        <v>0.9963479512055865</v>
+        <v>0.9963479512044059</v>
       </c>
       <c r="AZ7">
         <v>0</v>
       </c>
       <c r="BA7">
-        <v>0.003652048794413457</v>
+        <v>0.003652048795594057</v>
       </c>
       <c r="BB7">
         <v>0.9966639014863952</v>
@@ -2257,7 +2257,7 @@
         <v>0.993485592344309</v>
       </c>
       <c r="BU7">
-        <v>0.006514407655691032</v>
+        <v>0.006514407655691029</v>
       </c>
       <c r="BV7">
         <v>0</v>
@@ -2269,7 +2269,7 @@
         <v>0.9997663398579021</v>
       </c>
       <c r="BY7">
-        <v>0.000233660142097969</v>
+        <v>0.0002336601420979689</v>
       </c>
       <c r="BZ7">
         <v>0</v>

</xml_diff>